<commit_message>
Atualização automática de SOBRADINHO.xlsx
</commit_message>
<xml_diff>
--- a/SOBRADINHO.xlsx
+++ b/SOBRADINHO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66E9DEFB-774D-47DD-8F13-AEB496762279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E217ED1-17A3-43B0-BE9F-48470F2CF35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1197,7 +1197,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{90DF9847-6F1D-4A9A-97D3-05F5EAA43778}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{34385E18-7A51-4516-A015-B02E833E2F4B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1227,10 +1227,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{281D0929-9A2A-4AD2-8B59-A2FE1C35BA34}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62FE14BA-DCDD-44C5-B140-53B3564C0757}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1268,7 +1268,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FAB2F30-AFFE-4021-9D33-C2399526D8CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99A5B77C-3C0C-45F7-AAF7-534CC48C0CDF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1331,7 +1331,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1CC1FE5-6C56-4BCA-A2A7-31912E5891D3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54EA27DF-DA9C-48B4-9909-2CEB5DC353CD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1350,7 +1350,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EACD3F58-7431-0CD0-B1A4-A8C91D72220E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FAA9707-2402-9301-6DA8-904B4FB35D33}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1399,7 +1399,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E959315A-D9AD-31F9-A4EF-BC76A0F85C01}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5AC60D8-7D76-21AF-41CD-169B137B4D31}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1418,7 +1418,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A433621-0FC9-C406-7483-C031D891338F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AAA30EA-C86A-0AAC-0534-B196FA0B8F25}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1449,7 +1449,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91A01EE6-EDCA-3BCF-578D-8CA8D1CC4169}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADE5AB3F-25D6-1602-8778-4A3ED80A536D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1480,7 +1480,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2FD7263-238C-DB71-99F4-65CE1015E595}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01388A3F-FD48-7BDE-CDF4-73B3271694EF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1523,7 +1523,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA6EF031-68CF-4FE4-8084-A274A6B6F40E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A80D911A-A92F-4A99-AB9D-39682F3E7388}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1561,7 +1561,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B02AD93B-C010-4528-A9AC-F4BED46146D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9F578AA-80B3-4E12-A8F6-1DC46404F92E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1604,7 +1604,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{084E1667-6BC7-430A-B1BF-290000CF4419}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{329F9969-08D9-4EF0-8CAB-566373418485}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1917,7 +1917,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E3D61D6-EAEB-455E-A594-70F6F2CF664A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023E8771-0971-4C5E-A182-6FE15B7F76FE}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>